<commit_message>
ulteriori test sui dataset che hanno tutte le combinazioni (train set = test set)
</commit_message>
<xml_diff>
--- a/docs/Comparazione.xlsx
+++ b/docs/Comparazione.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Desktop\ALTRI DATASET\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Desktop\Davide\Altri\Università\A.A. 2021-2022\Rappresentazione della conoscenza\Progetto\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35EA258F-C063-42DF-99E7-94995D1E8F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{027A057A-29E2-49C2-A066-73470DF957DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12576" xr2:uid="{EF0F2243-DA28-4D26-A325-E2EFFD9F8778}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>DATASET</t>
   </si>
@@ -100,9 +100,6 @@
     <t>0.6666666666666666</t>
   </si>
   <si>
-    <t>yellow-small+adult-stretch</t>
-  </si>
-  <si>
     <t>0.9555555555555556</t>
   </si>
   <si>
@@ -187,12 +184,6 @@
     <t>0.810706787963611</t>
   </si>
   <si>
-    <t>study_cohort</t>
-  </si>
-  <si>
-    <t>Sono tutte le combinazioni</t>
-  </si>
-  <si>
     <t>0.6727162734422263</t>
   </si>
   <si>
@@ -200,6 +191,9 @@
   </si>
   <si>
     <t>0.38908327501749473</t>
+  </si>
+  <si>
+    <t>necessarie tutte le combinazioni</t>
   </si>
 </sst>
 </file>
@@ -604,7 +598,7 @@
     <col min="2" max="7" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -673,22 +667,22 @@
         <v>10</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>24</v>
-      </c>
       <c r="H3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="J3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K3" s="5"/>
     </row>
@@ -706,25 +700,25 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="H4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -750,13 +744,13 @@
         <v>15</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -773,96 +767,94 @@
         <v>19</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="H6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" t="s">
-        <v>21</v>
+        <v>32</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="J7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="I8" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>50</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="K8" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
modifica alla regola MRP3 + comparazione tra soglie per Sepsis
</commit_message>
<xml_diff>
--- a/docs/Comparazione.xlsx
+++ b/docs/Comparazione.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Desktop\Davide\Altri\Università\A.A. 2021-2022\Rappresentazione della conoscenza\Progetto\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D635598F-C408-42CF-8A75-430CAA6056A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0A5016-8010-41CF-891E-558ED2227F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
   <si>
     <t>DATASET</t>
   </si>
@@ -94,13 +94,19 @@
   </si>
   <si>
     <t>maximum recursion depth exceeded</t>
+  </si>
+  <si>
+    <t>&gt;2</t>
+  </si>
+  <si>
+    <t>Sepsis con MRP3 modificata (self test)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +184,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF24292F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -187,7 +199,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -314,18 +326,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -342,9 +401,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -378,6 +434,57 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -387,50 +494,27 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -746,509 +830,579 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231440DE-B0AD-45EC-A4AA-72D1E9D5737D}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="16" width="11.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="16" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2" t="s">
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="17" t="s">
+      <c r="B2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="17" t="s">
+      <c r="H2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="17" t="s">
+      <c r="K2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="18" t="s">
+      <c r="M2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" s="17" t="s">
+      <c r="N2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="18" t="s">
+      <c r="P2" s="16" t="s">
         <v>3</v>
       </c>
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="17">
         <v>0.94202898550000003</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>0.97744360900000005</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="18">
         <v>0.94444444439999997</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="17">
         <v>0.95555555560000005</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>0.96992481200000003</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="18">
         <v>0.95121951220000001</v>
       </c>
-      <c r="H3" s="19">
-        <v>1</v>
-      </c>
-      <c r="I3" s="5">
+      <c r="H3" s="17">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4">
         <v>0.59420289859999997</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="18">
         <v>0.4</v>
       </c>
-      <c r="K3" s="19">
-        <v>1</v>
-      </c>
-      <c r="L3" s="5">
+      <c r="K3" s="17">
+        <v>1</v>
+      </c>
+      <c r="L3" s="4">
         <v>0.79868708971553004</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="18">
         <v>0.55135951660000004</v>
       </c>
-      <c r="N3" s="19">
-        <v>1</v>
-      </c>
-      <c r="O3" s="5">
+      <c r="N3" s="17">
+        <v>1</v>
+      </c>
+      <c r="O3" s="4">
         <v>0.79868708971553004</v>
       </c>
-      <c r="P3" s="20">
+      <c r="P3" s="18">
         <v>0.55135951660000004</v>
       </c>
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="17">
         <v>0.99800399200000001</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.99800399200000001</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="18">
         <v>0.99791449430000001</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="17">
         <v>0.98051948050000004</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>0.98908296939999996</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="18">
         <v>0.98540145990000005</v>
       </c>
-      <c r="H4" s="27" t="s">
+      <c r="H4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="19">
-        <v>1</v>
-      </c>
-      <c r="L4" s="5">
+      <c r="K4" s="17">
+        <v>1</v>
+      </c>
+      <c r="L4" s="4">
         <v>0.96285200719999997</v>
       </c>
-      <c r="M4" s="20">
+      <c r="M4" s="18">
         <v>0.94962453069999997</v>
       </c>
-      <c r="N4" s="19">
-        <v>1</v>
-      </c>
-      <c r="O4" s="5">
+      <c r="N4" s="17">
+        <v>1</v>
+      </c>
+      <c r="O4" s="4">
         <v>0.96285200719999997</v>
       </c>
-      <c r="P4" s="20">
+      <c r="P4" s="18">
         <v>0.94962453069999997</v>
       </c>
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="19">
-        <v>1</v>
-      </c>
-      <c r="C5" s="5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="20">
-        <v>1</v>
-      </c>
-      <c r="E5" s="19">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5">
-        <v>1</v>
-      </c>
-      <c r="G5" s="20">
-        <v>1</v>
-      </c>
-      <c r="H5" s="19">
-        <v>1</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="B5" s="17">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="18">
+        <v>1</v>
+      </c>
+      <c r="E5" s="17">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="18">
+        <v>1</v>
+      </c>
+      <c r="H5" s="17">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4">
         <v>2.3330651649999999E-2</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="18">
         <v>1.9884009939999999E-2</v>
       </c>
-      <c r="K5" s="19">
-        <v>1</v>
-      </c>
-      <c r="L5" s="5">
+      <c r="K5" s="17">
+        <v>1</v>
+      </c>
+      <c r="L5" s="4">
         <v>0.99705882349999997</v>
       </c>
-      <c r="M5" s="20">
+      <c r="M5" s="18">
         <v>0.99848980620000005</v>
       </c>
-      <c r="N5" s="19">
-        <v>1</v>
-      </c>
-      <c r="O5" s="5">
+      <c r="N5" s="17">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4">
         <v>0.99705882349999997</v>
       </c>
-      <c r="P5" s="20">
+      <c r="P5" s="18">
         <v>0.99848980620000005</v>
       </c>
-      <c r="Q5" s="7"/>
+      <c r="Q5" s="6"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="17">
         <v>0.93918918920000005</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>0.97887323940000004</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="18">
         <v>0.97619047619999999</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="17">
         <v>0.88961038960000005</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>0.87820512819999996</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="18">
         <v>0.93063583819999995</v>
       </c>
-      <c r="H6" s="19">
-        <v>1</v>
-      </c>
-      <c r="I6" s="5">
+      <c r="H6" s="17">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4">
         <v>0.34285714290000002</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="18">
         <v>0.73575129530000005</v>
       </c>
-      <c r="K6" s="19">
-        <v>1</v>
-      </c>
-      <c r="L6" s="5">
-        <v>1</v>
-      </c>
-      <c r="M6" s="20">
-        <v>1</v>
-      </c>
-      <c r="N6" s="19">
-        <v>1</v>
-      </c>
-      <c r="O6" s="5">
-        <v>1</v>
-      </c>
-      <c r="P6" s="20">
+      <c r="K6" s="17">
+        <v>1</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1</v>
+      </c>
+      <c r="M6" s="18">
+        <v>1</v>
+      </c>
+      <c r="N6" s="17">
+        <v>1</v>
+      </c>
+      <c r="O6" s="4">
+        <v>1</v>
+      </c>
+      <c r="P6" s="18">
         <v>1</v>
       </c>
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24">
+      <c r="C7" s="37"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="19">
         <v>0.81070678799999996</v>
       </c>
-      <c r="F7" s="25">
-        <v>1</v>
-      </c>
-      <c r="G7" s="26">
+      <c r="F7" s="20">
+        <v>1</v>
+      </c>
+      <c r="G7" s="21">
         <v>0.81070678799999996</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="19">
         <v>0.89366053170000004</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="20">
         <v>9.4302977989999995E-2</v>
       </c>
-      <c r="J7" s="26">
+      <c r="J7" s="21">
         <v>7.8726382090000005E-2</v>
       </c>
-      <c r="K7" s="24">
+      <c r="K7" s="19">
         <v>0.99922540666150195</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="20">
         <v>8.352217546E-2</v>
       </c>
-      <c r="M7" s="26">
+      <c r="M7" s="21">
         <v>6.949766416E-2</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="19">
         <v>0.99922540666150195</v>
       </c>
-      <c r="O7" s="25">
+      <c r="O7" s="20">
         <v>8.352217546E-2</v>
       </c>
-      <c r="P7" s="26">
+      <c r="P7" s="21">
         <v>6.949766416E-2</v>
       </c>
       <c r="Q7" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:17" ht="27" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9" t="s">
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="8"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="7"/>
+      <c r="M11" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="34"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="34"/>
     </row>
     <row r="12" spans="1:17" ht="27" x14ac:dyDescent="0.3">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="27">
         <v>324</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="27">
         <v>420</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="27">
         <v>15588</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="37" t="s">
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="H12" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="8"/>
+      <c r="I12" s="7"/>
+      <c r="M12" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="48" t="s">
+        <v>1</v>
+      </c>
+      <c r="O12" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="P12" s="50" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="27">
         <v>495</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="27">
         <v>420</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="27">
         <v>65527</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="38">
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="33">
         <v>1000</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="9">
         <v>25648</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="I13" s="10" t="s">
         <v>21</v>
+      </c>
+      <c r="M13" s="40">
+        <v>0.9</v>
+      </c>
+      <c r="N13" s="43">
+        <v>0.811755952380952</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0.98892845581094202</v>
+      </c>
+      <c r="P13" s="44">
+        <v>0.80483964096372895</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="32">
+      <c r="B14" s="27">
         <v>105</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="27">
         <v>420</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="27">
         <v>29848</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="38">
-        <v>1</v>
-      </c>
-      <c r="H14" s="11">
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="33">
+        <v>1</v>
+      </c>
+      <c r="H14" s="9">
         <v>795557</v>
       </c>
-      <c r="I14" s="8"/>
+      <c r="I14" s="7"/>
+      <c r="M14" s="41">
+        <v>1</v>
+      </c>
+      <c r="N14" s="43">
+        <v>0.81182224112268697</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0.98879896406603995</v>
+      </c>
+      <c r="P14" s="44">
+        <v>0.80462967823211295</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="27">
         <v>755</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="27">
         <v>420</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="27">
         <v>819</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="38">
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="33">
         <v>0.9</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="9">
         <v>878378</v>
       </c>
-      <c r="I15" s="8"/>
+      <c r="I15" s="7"/>
+      <c r="M15" s="41">
+        <v>2</v>
+      </c>
+      <c r="N15" s="43">
+        <v>0.90507812499999996</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0.15001618646811199</v>
+      </c>
+      <c r="P15" s="44">
+        <v>0.12513778804262199</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="34">
+      <c r="C16" s="29">
         <v>420</v>
       </c>
-      <c r="D16" s="34">
+      <c r="D16" s="29">
         <v>7106</v>
       </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="38">
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="33">
         <v>0.5</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="9">
         <v>871763</v>
       </c>
-      <c r="I16" s="8"/>
+      <c r="I16" s="7"/>
+      <c r="M16" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="N16" s="45">
+        <v>0.99922540666150195</v>
+      </c>
+      <c r="O16" s="46">
+        <v>8.3522175461314296E-2</v>
+      </c>
+      <c r="P16" s="47">
+        <v>6.9497664164610701E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O17" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="B7:D7"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="B7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
aggiunti risultati test set 30% su Sepsis
</commit_message>
<xml_diff>
--- a/docs/Comparazione.xlsx
+++ b/docs/Comparazione.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Desktop\Davide\Altri\Università\A.A. 2021-2022\Rappresentazione della conoscenza\Progetto\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0A5016-8010-41CF-891E-558ED2227F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34299666-4781-4B80-9AEE-48A6E5277EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-13068" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>DATASET</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Algoritmo NMR (self test)</t>
   </si>
   <si>
-    <t>Algoritmo NMR (self test + Nlg(N)+ threashold=0.9)</t>
-  </si>
-  <si>
     <t>DIMENSIONE MODELLO</t>
   </si>
   <si>
@@ -81,15 +78,9 @@
     <t>MLP</t>
   </si>
   <si>
-    <t>NMR (self-test)</t>
-  </si>
-  <si>
     <t>Threshold</t>
   </si>
   <si>
-    <t>Numero di coppie</t>
-  </si>
-  <si>
     <t>(numero minimo di coppie)</t>
   </si>
   <si>
@@ -99,14 +90,29 @@
     <t>&gt;2</t>
   </si>
   <si>
-    <t>Sepsis con MRP3 modificata (self test)</t>
+    <t>Sepsis con MRP3 nuova (test set 30%)</t>
+  </si>
+  <si>
+    <t>Sepsis con MRP3 nuova (self test)</t>
+  </si>
+  <si>
+    <t>THRESHOLD</t>
+  </si>
+  <si>
+    <t>NMR (self test)</t>
+  </si>
+  <si>
+    <t>#coppie</t>
+  </si>
+  <si>
+    <t>Algoritmo NMR (self test + Nlg(N) + threshold=0,9)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +196,14 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -199,7 +213,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -219,26 +233,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -330,19 +324,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -380,7 +361,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -413,71 +394,79 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -485,36 +474,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -830,7 +808,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{231440DE-B0AD-45EC-A4AA-72D1E9D5737D}">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -843,80 +821,80 @@
   <sheetData>
     <row r="1" spans="1:17" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35" t="s">
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="41"/>
+      <c r="P1" s="41"/>
       <c r="Q1" s="1"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="15" t="s">
+      <c r="E2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="15" t="s">
+      <c r="H2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="15" t="s">
+      <c r="K2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" s="15" t="s">
+      <c r="N2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="39" t="s">
         <v>3</v>
       </c>
       <c r="Q2" s="1"/>
@@ -925,49 +903,49 @@
       <c r="A3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="14">
         <v>0.94202898550000003</v>
       </c>
       <c r="C3" s="4">
         <v>0.97744360900000005</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="15">
         <v>0.94444444439999997</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="14">
         <v>0.95555555560000005</v>
       </c>
       <c r="F3" s="4">
         <v>0.96992481200000003</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="15">
         <v>0.95121951220000001</v>
       </c>
-      <c r="H3" s="17">
+      <c r="H3" s="14">
         <v>1</v>
       </c>
       <c r="I3" s="4">
         <v>0.59420289859999997</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="15">
         <v>0.4</v>
       </c>
-      <c r="K3" s="17">
+      <c r="K3" s="14">
         <v>1</v>
       </c>
       <c r="L3" s="4">
         <v>0.79868708971553004</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="15">
         <v>0.55135951660000004</v>
       </c>
-      <c r="N3" s="17">
+      <c r="N3" s="14">
         <v>1</v>
       </c>
       <c r="O3" s="4">
         <v>0.79868708971553004</v>
       </c>
-      <c r="P3" s="18">
+      <c r="P3" s="15">
         <v>0.55135951660000004</v>
       </c>
       <c r="Q3" s="1"/>
@@ -976,49 +954,49 @@
       <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="14">
         <v>0.99800399200000001</v>
       </c>
       <c r="C4" s="4">
         <v>0.99800399200000001</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="15">
         <v>0.99791449430000001</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="14">
         <v>0.98051948050000004</v>
       </c>
       <c r="F4" s="4">
         <v>0.98908296939999996</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="15">
         <v>0.98540145990000005</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="19" t="s">
         <v>9</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K4" s="14">
         <v>1</v>
       </c>
       <c r="L4" s="4">
         <v>0.96285200719999997</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="15">
         <v>0.94962453069999997</v>
       </c>
-      <c r="N4" s="17">
+      <c r="N4" s="14">
         <v>1</v>
       </c>
       <c r="O4" s="4">
         <v>0.96285200719999997</v>
       </c>
-      <c r="P4" s="18">
+      <c r="P4" s="15">
         <v>0.94962453069999997</v>
       </c>
       <c r="Q4" s="1"/>
@@ -1027,49 +1005,49 @@
       <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="14">
         <v>1</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="18">
-        <v>1</v>
-      </c>
-      <c r="E5" s="17">
+      <c r="D5" s="15">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
         <v>1</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
       </c>
-      <c r="G5" s="18">
-        <v>1</v>
-      </c>
-      <c r="H5" s="17">
+      <c r="G5" s="15">
+        <v>1</v>
+      </c>
+      <c r="H5" s="14">
         <v>1</v>
       </c>
       <c r="I5" s="4">
         <v>2.3330651649999999E-2</v>
       </c>
-      <c r="J5" s="18">
+      <c r="J5" s="15">
         <v>1.9884009939999999E-2</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="14">
         <v>1</v>
       </c>
       <c r="L5" s="4">
         <v>0.99705882349999997</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="15">
         <v>0.99848980620000005</v>
       </c>
-      <c r="N5" s="17">
+      <c r="N5" s="14">
         <v>1</v>
       </c>
       <c r="O5" s="4">
         <v>0.99705882349999997</v>
       </c>
-      <c r="P5" s="18">
+      <c r="P5" s="15">
         <v>0.99848980620000005</v>
       </c>
       <c r="Q5" s="6"/>
@@ -1078,49 +1056,49 @@
       <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="14">
         <v>0.93918918920000005</v>
       </c>
       <c r="C6" s="4">
         <v>0.97887323940000004</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="15">
         <v>0.97619047619999999</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="14">
         <v>0.88961038960000005</v>
       </c>
       <c r="F6" s="4">
         <v>0.87820512819999996</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="15">
         <v>0.93063583819999995</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H6" s="14">
         <v>1</v>
       </c>
       <c r="I6" s="4">
         <v>0.34285714290000002</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="15">
         <v>0.73575129530000005</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6" s="14">
         <v>1</v>
       </c>
       <c r="L6" s="4">
         <v>1</v>
       </c>
-      <c r="M6" s="18">
-        <v>1</v>
-      </c>
-      <c r="N6" s="17">
+      <c r="M6" s="15">
+        <v>1</v>
+      </c>
+      <c r="N6" s="14">
         <v>1</v>
       </c>
       <c r="O6" s="4">
         <v>1</v>
       </c>
-      <c r="P6" s="18">
+      <c r="P6" s="15">
         <v>1</v>
       </c>
       <c r="Q6" s="1"/>
@@ -1129,56 +1107,56 @@
       <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="19">
+      <c r="B7" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="16">
         <v>0.81070678799999996</v>
       </c>
-      <c r="F7" s="20">
-        <v>1</v>
-      </c>
-      <c r="G7" s="21">
+      <c r="F7" s="17">
+        <v>1</v>
+      </c>
+      <c r="G7" s="18">
         <v>0.81070678799999996</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="16">
         <v>0.89366053170000004</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="17">
         <v>9.4302977989999995E-2</v>
       </c>
-      <c r="J7" s="21">
+      <c r="J7" s="18">
         <v>7.8726382090000005E-2</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="16">
         <v>0.99922540666150195</v>
       </c>
-      <c r="L7" s="20">
+      <c r="L7" s="17">
         <v>8.352217546E-2</v>
       </c>
-      <c r="M7" s="21">
+      <c r="M7" s="18">
         <v>6.949766416E-2</v>
       </c>
-      <c r="N7" s="19">
+      <c r="N7" s="16">
         <v>0.99922540666150195</v>
       </c>
-      <c r="O7" s="20">
+      <c r="O7" s="17">
         <v>8.352217546E-2</v>
       </c>
-      <c r="P7" s="21">
+      <c r="P7" s="18">
         <v>6.949766416E-2</v>
       </c>
       <c r="Q7" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
-      <c r="B10" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
+      <c r="B10" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -1189,220 +1167,277 @@
       <c r="A11" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="D11" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="40"/>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="24">
+        <v>324</v>
+      </c>
+      <c r="C12" s="24">
+        <v>420</v>
+      </c>
+      <c r="D12" s="24">
+        <v>15588</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="G12" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="24">
+        <v>495</v>
+      </c>
+      <c r="C13" s="24">
+        <v>420</v>
+      </c>
+      <c r="D13" s="24">
+        <v>65527</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="30">
+        <v>1000</v>
+      </c>
+      <c r="G13" s="9">
+        <v>25648</v>
+      </c>
+      <c r="H13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="34" t="s">
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="24">
+        <v>105</v>
+      </c>
+      <c r="C14" s="24">
+        <v>420</v>
+      </c>
+      <c r="D14" s="24">
+        <v>29848</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="30">
+        <v>1</v>
+      </c>
+      <c r="G14" s="9">
+        <v>795557</v>
+      </c>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="24">
+        <v>755</v>
+      </c>
+      <c r="C15" s="24">
+        <v>420</v>
+      </c>
+      <c r="D15" s="24">
+        <v>819</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="30">
+        <v>0.9</v>
+      </c>
+      <c r="G15" s="9">
+        <v>878378</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="34"/>
-      <c r="I11" s="7"/>
-      <c r="M11" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-    </row>
-    <row r="12" spans="1:17" ht="27" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="27">
-        <v>324</v>
-      </c>
-      <c r="C12" s="27">
+      <c r="B16" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="26">
         <v>420</v>
       </c>
-      <c r="D12" s="27">
-        <v>15588</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="31" t="s">
+      <c r="D16" s="26">
+        <v>7106</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="G16" s="9">
+        <v>871763</v>
+      </c>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O17" s="31"/>
+    </row>
+    <row r="19" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="45"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="47">
+        <v>0.9</v>
+      </c>
+      <c r="B21" s="32">
+        <v>0.80948995912564403</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.98295209322399602</v>
+      </c>
+      <c r="D21" s="33">
+        <v>0.79706088173547895</v>
+      </c>
+      <c r="E21" s="32">
+        <v>0.811755952380952</v>
+      </c>
+      <c r="F21" s="2">
+        <v>0.98892845581094202</v>
+      </c>
+      <c r="G21" s="33">
+        <v>0.80483964096372895</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="48">
+        <v>1</v>
+      </c>
+      <c r="B22" s="32">
+        <v>0.80948995912564403</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.98295209322399602</v>
+      </c>
+      <c r="D22" s="33">
+        <v>0.79706088173547895</v>
+      </c>
+      <c r="E22" s="32">
+        <v>0.81182224112268697</v>
+      </c>
+      <c r="F22" s="2">
+        <v>0.98879896406603995</v>
+      </c>
+      <c r="G22" s="33">
+        <v>0.80462967823211295</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="48">
+        <v>2</v>
+      </c>
+      <c r="B23" s="32">
+        <v>0.85336048879837001</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.180837289598618</v>
+      </c>
+      <c r="D23" s="33">
+        <v>0.14835549335199399</v>
+      </c>
+      <c r="E23" s="32">
+        <v>0.90507812499999996</v>
+      </c>
+      <c r="F23" s="2">
+        <v>0.15001618646811199</v>
+      </c>
+      <c r="G23" s="33">
+        <v>0.12513778804262199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="M12" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="N12" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="O12" s="49" t="s">
-        <v>2</v>
-      </c>
-      <c r="P12" s="50" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="27">
-        <v>495</v>
-      </c>
-      <c r="C13" s="27">
-        <v>420</v>
-      </c>
-      <c r="D13" s="27">
-        <v>65527</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="33">
-        <v>1000</v>
-      </c>
-      <c r="H13" s="9">
-        <v>25648</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="40">
-        <v>0.9</v>
-      </c>
-      <c r="N13" s="43">
-        <v>0.811755952380952</v>
-      </c>
-      <c r="O13" s="2">
-        <v>0.98892845581094202</v>
-      </c>
-      <c r="P13" s="44">
-        <v>0.80483964096372895</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="27">
-        <v>105</v>
-      </c>
-      <c r="C14" s="27">
-        <v>420</v>
-      </c>
-      <c r="D14" s="27">
-        <v>29848</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="33">
-        <v>1</v>
-      </c>
-      <c r="H14" s="9">
-        <v>795557</v>
-      </c>
-      <c r="I14" s="7"/>
-      <c r="M14" s="41">
-        <v>1</v>
-      </c>
-      <c r="N14" s="43">
-        <v>0.81182224112268697</v>
-      </c>
-      <c r="O14" s="2">
-        <v>0.98879896406603995</v>
-      </c>
-      <c r="P14" s="44">
-        <v>0.80462967823211295</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="27">
-        <v>755</v>
-      </c>
-      <c r="C15" s="27">
-        <v>420</v>
-      </c>
-      <c r="D15" s="27">
-        <v>819</v>
-      </c>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="33">
-        <v>0.9</v>
-      </c>
-      <c r="H15" s="9">
-        <v>878378</v>
-      </c>
-      <c r="I15" s="7"/>
-      <c r="M15" s="41">
-        <v>2</v>
-      </c>
-      <c r="N15" s="43">
-        <v>0.90507812499999996</v>
-      </c>
-      <c r="O15" s="2">
-        <v>0.15001618646811199</v>
-      </c>
-      <c r="P15" s="44">
-        <v>0.12513778804262199</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="29">
-        <v>420</v>
-      </c>
-      <c r="D16" s="29">
-        <v>7106</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="33">
-        <v>0.5</v>
-      </c>
-      <c r="H16" s="9">
-        <v>871763</v>
-      </c>
-      <c r="I16" s="7"/>
-      <c r="M16" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="N16" s="45">
+      <c r="B24" s="34">
+        <v>0.89366053169734105</v>
+      </c>
+      <c r="C24" s="35">
+        <v>9.4302977988778597E-2</v>
+      </c>
+      <c r="D24" s="36">
+        <v>7.8726382085374302E-2</v>
+      </c>
+      <c r="E24" s="34">
         <v>0.99922540666150195</v>
       </c>
-      <c r="O16" s="46">
+      <c r="F24" s="35">
         <v>8.3522175461314296E-2</v>
       </c>
-      <c r="P16" s="47">
+      <c r="G24" s="36">
         <v>6.9497664164610701E-2</v>
       </c>
     </row>
-    <row r="17" spans="15:15" x14ac:dyDescent="0.3">
-      <c r="O17" s="39"/>
-    </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="M11:P11"/>
+  <mergeCells count="10">
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="B7:D7"/>
     <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G11:H11"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="F11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>